<commit_message>
1. Added Idle loop to track pressure in real time 2. Added Emergency Depressurize Loop in case door opens when bottle is being pressurized 3. Added spreadsheet with version control and configuration control data
</commit_message>
<xml_diff>
--- a/Component Configuration.xlsx
+++ b/Component Configuration.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Touchsensor capacitive touchbuttons</t>
   </si>
@@ -24,9 +24,6 @@
     <t>Arduino MICRO Controller</t>
   </si>
   <si>
-    <t>5 Normally Closed solenoids</t>
-  </si>
-  <si>
     <t>Sainsmart 8-channel relay</t>
   </si>
   <si>
@@ -43,6 +40,93 @@
   </si>
   <si>
     <t>PCB v1</t>
+  </si>
+  <si>
+    <t>Normally Closed solenoids</t>
+  </si>
+  <si>
+    <t>First version w/ custom lift</t>
+  </si>
+  <si>
+    <t>Demo'd at Tales</t>
+  </si>
+  <si>
+    <t>Multiple corrections/refinements of v2.0</t>
+  </si>
+  <si>
+    <t>Not built</t>
+  </si>
+  <si>
+    <t>First unibody design</t>
+  </si>
+  <si>
+    <t>swapped out custom lift for dual rail cylinder</t>
+  </si>
+  <si>
+    <t>Taller; touchbuttons</t>
+  </si>
+  <si>
+    <t>w/ Micro</t>
+  </si>
+  <si>
+    <t>v3.0 w/ safety door added</t>
+  </si>
+  <si>
+    <t>Commenst</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Component</t>
+  </si>
+  <si>
+    <t>added right before TOTC</t>
+  </si>
+  <si>
+    <t>New features or significant fixes (2nd digit)</t>
+  </si>
+  <si>
+    <t>Any change in hardware that breaks compatibility with firmware is a major revision (1st digit)</t>
+  </si>
+  <si>
+    <t>Hotfixes (3rd digit)</t>
+  </si>
+  <si>
+    <t>Any change in sheet metal or manufactured components that affects anything else is a significant revision (2nd digit)</t>
+  </si>
+  <si>
+    <t>Any change in purchased or manufactured components that affect nothing else is a minor revsion (3rd digit)</t>
+  </si>
+  <si>
+    <t>v0.1.0.0</t>
+  </si>
+  <si>
+    <t>v0.1.0.1</t>
+  </si>
+  <si>
+    <t>v0.2.0.0</t>
+  </si>
+  <si>
+    <t>v0.2.1.0</t>
+  </si>
+  <si>
+    <t>v0.3.0.0</t>
+  </si>
+  <si>
+    <t>v0.4.0.0</t>
+  </si>
+  <si>
+    <t>Leading zero means pre-release. First release will be v1.0.0</t>
+  </si>
+  <si>
+    <t>Software will be versioned by build number</t>
+  </si>
+  <si>
+    <t>Instructions for versioning</t>
   </si>
 </sst>
 </file>
@@ -93,11 +177,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -392,82 +482,242 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="41.7109375" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="5"/>
+    <col min="2" max="2" width="41.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="67.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="18.75">
       <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="3" customFormat="1">
+      <c r="A2" s="4"/>
+    </row>
+    <row r="3" spans="1:4" s="3" customFormat="1">
+      <c r="A3" s="4"/>
+      <c r="B3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" s="3" customFormat="1">
-      <c r="B2" s="3" t="s">
+      <c r="D3" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="5">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
+      <c r="C4" s="2">
+        <v>41644</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2">
+        <v>41944</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="5">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2">
+        <v>41456</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="5">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="2">
-        <v>41649</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
+      <c r="C7" s="2">
+        <v>41395</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="5">
         <v>1</v>
       </c>
-      <c r="B4" s="2">
-        <v>41649</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="2">
-        <v>41649</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
+      <c r="B8" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="2">
-        <v>41649</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
+      <c r="C8" s="2">
+        <v>41395</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="5">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="2">
-        <v>41649</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
+      <c r="C9" s="2">
+        <v>41395</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="5">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="2">
-        <v>41649</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="2">
-        <v>41649</v>
+      <c r="C10" s="2">
+        <v>41440</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="3" customFormat="1">
+      <c r="A13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="3" customFormat="1">
+      <c r="A14" s="4"/>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="2">
+        <v>41409</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="2">
+        <v>41440</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="2">
+        <v>41470</v>
+      </c>
+      <c r="D17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="2">
+        <v>41501</v>
+      </c>
+      <c r="D18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="2">
+        <v>41562</v>
+      </c>
+      <c r="D19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="2">
+        <v>41640</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" s="3" customFormat="1">
+      <c r="A23" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="B30" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1) Minor changes to comments 2) Rev'd version doc
</commit_message>
<xml_diff>
--- a/Component Configuration.xlsx
+++ b/Component Configuration.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
   <si>
     <t>Touchsensor capacitive touchbuttons</t>
   </si>
@@ -36,9 +36,6 @@
     <t>PBS Components that Affect Firmware</t>
   </si>
   <si>
-    <t>Date Added</t>
-  </si>
-  <si>
     <t>PCB v1</t>
   </si>
   <si>
@@ -72,9 +69,6 @@
     <t>v3.0 w/ safety door added</t>
   </si>
   <si>
-    <t>Commenst</t>
-  </si>
-  <si>
     <t>Version</t>
   </si>
   <si>
@@ -127,6 +121,24 @@
   </si>
   <si>
     <t>Instructions for versioning</t>
+  </si>
+  <si>
+    <t>Cleaning switch moved from J10 to J11</t>
+  </si>
+  <si>
+    <t>v0.5.0.0</t>
+  </si>
+  <si>
+    <t>Cleaning switch now logic controlled</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>No.</t>
+  </si>
+  <si>
+    <t>Comments</t>
   </si>
 </sst>
 </file>
@@ -177,7 +189,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -187,6 +199,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -482,7 +504,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -490,7 +512,7 @@
   <cols>
     <col min="1" max="1" width="9.140625" style="5"/>
     <col min="2" max="2" width="41.7109375" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" style="2" customWidth="1"/>
     <col min="4" max="4" width="67.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -498,31 +520,33 @@
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="C1" s="8"/>
     </row>
     <row r="2" spans="1:4" s="3" customFormat="1">
       <c r="A2" s="4"/>
+      <c r="C2" s="9"/>
     </row>
     <row r="3" spans="1:4" s="3" customFormat="1">
-      <c r="A3" s="4"/>
+      <c r="A3" s="4" t="s">
+        <v>39</v>
+      </c>
       <c r="B3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>6</v>
+        <v>19</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>38</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="5">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="2">
-        <v>41644</v>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="7" customFormat="1">
+      <c r="A4" s="6"/>
+      <c r="B4" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="10">
+        <v>41659</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -530,10 +554,10 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C5" s="2">
-        <v>41944</v>
+        <v>41644</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -541,32 +565,32 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" s="2">
-        <v>41456</v>
-      </c>
-      <c r="D6" t="s">
-        <v>22</v>
+        <v>41944</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="5">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C7" s="2">
-        <v>41395</v>
+        <v>41456</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C8" s="2">
         <v>41395</v>
@@ -577,7 +601,7 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C9" s="2">
         <v>41395</v>
@@ -588,136 +612,167 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="2">
+        <v>41395</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="5">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C11" s="2">
         <v>41440</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="3" customFormat="1">
-      <c r="A13" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
     <row r="14" spans="1:4" s="3" customFormat="1">
-      <c r="A14" s="4"/>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="2">
-        <v>41409</v>
-      </c>
+      <c r="A14" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="3" customFormat="1">
+      <c r="A15" s="4"/>
+      <c r="C15" s="9"/>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C16" s="2">
-        <v>41440</v>
+        <v>41409</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B17" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C17" s="2">
-        <v>41470</v>
-      </c>
-      <c r="D17" t="s">
-        <v>15</v>
+        <v>41440</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B18" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C18" s="2">
-        <v>41501</v>
+        <v>41470</v>
       </c>
       <c r="D18" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B19" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C19" s="2">
-        <v>41562</v>
+        <v>41501</v>
       </c>
       <c r="D19" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B20" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C20" s="2">
+        <v>41562</v>
+      </c>
+      <c r="D20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="2">
         <v>41640</v>
       </c>
     </row>
-    <row r="23" spans="1:4" s="3" customFormat="1">
-      <c r="A23" s="4" t="s">
+    <row r="22" spans="1:4">
+      <c r="A22" s="5" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" t="s">
+      <c r="B22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="2">
+        <v>41659</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" s="3" customFormat="1">
+      <c r="A25" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" t="s">
-        <v>26</v>
-      </c>
+      <c r="C25" s="9"/>
+    </row>
+    <row r="26" spans="1:4" s="3" customFormat="1">
+      <c r="A26" s="4"/>
+      <c r="C26" s="9"/>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
-      <c r="B30" t="s">
-        <v>35</v>
+    <row r="31" spans="1:4">
+      <c r="A31" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1. First shot at menu design
</commit_message>
<xml_diff>
--- a/Component Configuration.xlsx
+++ b/Component Configuration.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
   <si>
     <t>Touchsensor capacitive touchbuttons</t>
   </si>
@@ -81,21 +81,6 @@
     <t>added right before TOTC</t>
   </si>
   <si>
-    <t>New features or significant fixes (2nd digit)</t>
-  </si>
-  <si>
-    <t>Any change in hardware that breaks compatibility with firmware is a major revision (1st digit)</t>
-  </si>
-  <si>
-    <t>Hotfixes (3rd digit)</t>
-  </si>
-  <si>
-    <t>Any change in sheet metal or manufactured components that affects anything else is a significant revision (2nd digit)</t>
-  </si>
-  <si>
-    <t>Any change in purchased or manufactured components that affect nothing else is a minor revsion (3rd digit)</t>
-  </si>
-  <si>
     <t>v0.1.0.0</t>
   </si>
   <si>
@@ -117,9 +102,6 @@
     <t>Leading zero means pre-release. First release will be v1.0.0</t>
   </si>
   <si>
-    <t>Software will be versioned by build number</t>
-  </si>
-  <si>
     <t>Instructions for versioning</t>
   </si>
   <si>
@@ -129,9 +111,6 @@
     <t>v0.5.0.0</t>
   </si>
   <si>
-    <t>Cleaning switch now logic controlled</t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
@@ -139,6 +118,36 @@
   </si>
   <si>
     <t>Comments</t>
+  </si>
+  <si>
+    <t>Cleaning switch added</t>
+  </si>
+  <si>
+    <t>This is logic controlled; so breaks backwards compatibility</t>
+  </si>
+  <si>
+    <t>Hardware</t>
+  </si>
+  <si>
+    <t>Software</t>
+  </si>
+  <si>
+    <t>1st digit same as first hardware version digit</t>
+  </si>
+  <si>
+    <t>2nd digit represents new features or major bugs</t>
+  </si>
+  <si>
+    <t>3rd digit is for minor hot fixes</t>
+  </si>
+  <si>
+    <t>1st digit: Any change in hardware that breaks compatibility with firmware is a major revision and increments 1st digit</t>
+  </si>
+  <si>
+    <t>2nd digit: Any change in sheet metal or manufactured components that affects anything else is a significant revision and increments 2nd digit</t>
+  </si>
+  <si>
+    <t>3rd digit: Any change in purchased or manufactured components that affect nothing else is a minor revsion and increments 3rd digit</t>
   </si>
 </sst>
 </file>
@@ -504,7 +513,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -528,22 +537,22 @@
     </row>
     <row r="3" spans="1:4" s="3" customFormat="1">
       <c r="A3" s="4" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="7" customFormat="1">
       <c r="A4" s="6"/>
       <c r="B4" s="7" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C4" s="10">
         <v>41659</v>
@@ -637,7 +646,7 @@
         <v>18</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:4" s="3" customFormat="1">
@@ -646,7 +655,7 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="5" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B16" t="s">
         <v>8</v>
@@ -657,7 +666,7 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B17" t="s">
         <v>13</v>
@@ -668,7 +677,7 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B18" t="s">
         <v>9</v>
@@ -682,7 +691,7 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B19" t="s">
         <v>10</v>
@@ -696,7 +705,7 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B20" t="s">
         <v>12</v>
@@ -710,7 +719,7 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B21" t="s">
         <v>16</v>
@@ -721,59 +730,82 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="5" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B22" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C22" s="2">
         <v>41659</v>
       </c>
+      <c r="D22" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="25" spans="1:4" s="3" customFormat="1">
       <c r="A25" s="4" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C25" s="9"/>
     </row>
     <row r="26" spans="1:4" s="3" customFormat="1">
-      <c r="A26" s="4"/>
+      <c r="A26" s="4" t="s">
+        <v>36</v>
+      </c>
       <c r="C26" s="9"/>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1">
+      <c r="A31"/>
+    </row>
+    <row r="32" spans="1:4" s="3" customFormat="1">
+      <c r="A32" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32" s="9"/>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" s="7" customFormat="1">
       <c r="A34" t="s">
-        <v>33</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="C34" s="10"/>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>